<commit_message>
Version 1.0 All modes added moving to master branch
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Mode1" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Phase Name</t>
+  </si>
+  <si>
+    <t>Data Points</t>
+  </si>
   <si>
     <t>Preliminary Design</t>
   </si>
@@ -36,6 +48,9 @@
   </si>
   <si>
     <t>System Test</t>
+  </si>
+  <si>
+    <t>Defects Detected</t>
   </si>
   <si>
     <t>HLD</t>
@@ -150,10 +165,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B6"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -163,40 +178,40 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B1" s="0" t="n">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>15</v>
@@ -204,79 +219,79 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>34</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>67</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>41</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>71</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>80</v>
@@ -284,55 +299,55 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>42</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>60</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>92</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>31</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>68</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>51</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>51</v>
@@ -340,89 +355,97 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>30</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="B33" s="0" t="n">
+      <c r="B34" s="0" t="n">
         <v>15</v>
       </c>
     </row>
@@ -442,10 +465,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B6"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -454,51 +477,59 @@
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="n">
         <v>20</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B6" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="0" t="n">
         <v>26</v>
       </c>
     </row>
@@ -518,10 +549,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -532,49 +563,57 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B6" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="0" t="n">
         <v>26</v>
       </c>
     </row>
@@ -594,10 +633,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -607,49 +646,57 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>10.2</v>
+        <v>2</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>6.32</v>
+        <v>10.2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>7.48</v>
+        <v>6.32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>6.27</v>
+        <v>7.48</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>4.07</v>
+        <v>6.27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B6" s="0" t="n">
+        <v>4.07</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="0" t="n">
         <v>2.11</v>
       </c>
     </row>

</xml_diff>